<commit_message>
Fixed bug in landscape_values (maes ecosystem names not correct)
</commit_message>
<xml_diff>
--- a/data-raw/landscape_values_raw.xlsx
+++ b/data-raw/landscape_values_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/ecoservr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_AD4D5CB4E552A5DACE1C64C0901D4AE65BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B79CEB20-BC64-4DA9-9542-90CE7F22F994}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_AD4D5CB4E552A5DACE1C64C0901D4AE65BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9746151-8B38-489B-B3D0-949161357BCC}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="315" windowWidth="12900" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Prati stabili (foraggere permanenti)</t>
   </si>
   <si>
-    <t>Grassland</t>
-  </si>
-  <si>
     <t>Annual crops associated with permanent crops</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>Boschi misti di conifere e latifoglie</t>
   </si>
   <si>
-    <t>Natural grassland</t>
-  </si>
-  <si>
     <t>Aree a pascolo naturale e praterie</t>
   </si>
   <si>
@@ -361,6 +355,12 @@
   </si>
   <si>
     <t>Marine</t>
+  </si>
+  <si>
+    <t>Grasslands</t>
+  </si>
+  <si>
+    <t>Natural Grasslands</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1087,7 @@
         <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="E19">
         <v>331</v>
@@ -1110,10 +1110,10 @@
         <v>241</v>
       </c>
       <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
@@ -1139,10 +1139,10 @@
         <v>242</v>
       </c>
       <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -1168,10 +1168,10 @@
         <v>243</v>
       </c>
       <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
         <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>56</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
@@ -1197,10 +1197,10 @@
         <v>244</v>
       </c>
       <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
         <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -1226,28 +1226,28 @@
         <v>311</v>
       </c>
       <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
         <v>59</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>60</v>
-      </c>
-      <c r="D24" t="s">
-        <v>61</v>
       </c>
       <c r="E24">
         <v>254</v>
       </c>
       <c r="F24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" t="s">
         <v>62</v>
-      </c>
-      <c r="G24" t="s">
-        <v>63</v>
       </c>
       <c r="H24">
         <v>2007</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1255,28 +1255,28 @@
         <v>312</v>
       </c>
       <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
         <v>65</v>
       </c>
-      <c r="C25" t="s">
-        <v>66</v>
-      </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25">
         <v>254</v>
       </c>
       <c r="F25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" t="s">
         <v>62</v>
-      </c>
-      <c r="G25" t="s">
-        <v>63</v>
       </c>
       <c r="H25">
         <v>2007</v>
       </c>
       <c r="I25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1284,28 +1284,28 @@
         <v>313</v>
       </c>
       <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
         <v>67</v>
       </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26">
         <v>254</v>
       </c>
       <c r="F26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" t="s">
         <v>62</v>
-      </c>
-      <c r="G26" t="s">
-        <v>63</v>
       </c>
       <c r="H26">
         <v>2007</v>
       </c>
       <c r="I26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1313,13 +1313,13 @@
         <v>321</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="E27">
         <v>331</v>
@@ -1342,28 +1342,28 @@
         <v>322</v>
       </c>
       <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s">
         <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
       </c>
       <c r="E28">
         <v>254</v>
       </c>
       <c r="F28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" t="s">
         <v>62</v>
-      </c>
-      <c r="G28" t="s">
-        <v>63</v>
       </c>
       <c r="H28">
         <v>2007</v>
       </c>
       <c r="I28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1371,28 +1371,28 @@
         <v>323</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29">
         <v>254</v>
       </c>
       <c r="F29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" t="s">
         <v>62</v>
-      </c>
-      <c r="G29" t="s">
-        <v>63</v>
       </c>
       <c r="H29">
         <v>2007</v>
       </c>
       <c r="I29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1400,28 +1400,28 @@
         <v>324</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30">
         <v>254</v>
       </c>
       <c r="F30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" t="s">
         <v>62</v>
-      </c>
-      <c r="G30" t="s">
-        <v>63</v>
       </c>
       <c r="H30">
         <v>2007</v>
       </c>
       <c r="I30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1429,13 +1429,13 @@
         <v>331</v>
       </c>
       <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
         <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1446,13 +1446,13 @@
         <v>332</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1463,13 +1463,13 @@
         <v>333</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1480,13 +1480,13 @@
         <v>334</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1497,13 +1497,13 @@
         <v>335</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1514,13 +1514,13 @@
         <v>411</v>
       </c>
       <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" t="s">
         <v>88</v>
-      </c>
-      <c r="C36" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" t="s">
-        <v>90</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1531,13 +1531,13 @@
         <v>412</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1548,13 +1548,13 @@
         <v>421</v>
       </c>
       <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
         <v>93</v>
-      </c>
-      <c r="C38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" t="s">
-        <v>95</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1565,13 +1565,13 @@
         <v>422</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1582,13 +1582,13 @@
         <v>423</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1599,13 +1599,13 @@
         <v>511</v>
       </c>
       <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" t="s">
         <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" t="s">
-        <v>102</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1616,13 +1616,13 @@
         <v>512</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1633,13 +1633,13 @@
         <v>521</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1650,13 +1650,13 @@
         <v>522</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1667,13 +1667,13 @@
         <v>523</v>
       </c>
       <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
         <v>109</v>
-      </c>
-      <c r="C45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" t="s">
-        <v>111</v>
       </c>
       <c r="E45">
         <v>0</v>

</xml_diff>